<commit_message>
added pending works as of 3/24/18
</commit_message>
<xml_diff>
--- a/SMYDATA Sprint 1.xlsx
+++ b/SMYDATA Sprint 1.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint - 1" sheetId="4" r:id="rId1"/>
     <sheet name="Queries" sheetId="5" r:id="rId2"/>
     <sheet name="GAPS" sheetId="6" r:id="rId3"/>
     <sheet name="FLOW" sheetId="7" r:id="rId4"/>
+    <sheet name="Dilip" sheetId="8" r:id="rId5"/>
+    <sheet name="Parthiya" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="153">
   <si>
     <t>SL.NO</t>
   </si>
@@ -428,6 +430,54 @@
   </si>
   <si>
     <t>Multiple business, with more number of shops</t>
+  </si>
+  <si>
+    <t>Pending Works</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location </t>
+  </si>
+  <si>
+    <t>get latitude and longitude</t>
+  </si>
+  <si>
+    <t>validations</t>
+  </si>
+  <si>
+    <t>id proof attachment</t>
+  </si>
+  <si>
+    <t>input validations, password required length,email id , mobile ,pin code, reg id.</t>
+  </si>
+  <si>
+    <t>otp number</t>
+  </si>
+  <si>
+    <t>only numbers are allowed to enter in  OTP input</t>
+  </si>
+  <si>
+    <t>resend otp</t>
+  </si>
+  <si>
+    <t>how many times user allowed to ask for resend??</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forgot pswd and sign up </t>
+  </si>
+  <si>
+    <t>sign Up Page and addNew business and edit myInfo</t>
+  </si>
+  <si>
+    <t>Sl.No</t>
+  </si>
+  <si>
+    <t>Business category cannot able to change</t>
+  </si>
+  <si>
+    <t>Edit my Info</t>
+  </si>
+  <si>
+    <t>Business ID cannot able to change</t>
   </si>
 </sst>
 </file>
@@ -502,7 +552,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -560,6 +610,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,7 +680,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -637,9 +693,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -647,9 +700,6 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -680,6 +730,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -992,54 +1052,54 @@
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" customWidth="1"/>
-    <col min="11" max="11" width="31.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1047,161 +1107,161 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G3" s="26">
         <v>43167</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H3" s="26">
         <v>43174</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="11" t="s">
+      <c r="I3" s="27"/>
+      <c r="J3" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="30"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="31" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="28">
+      <c r="F4" s="29"/>
+      <c r="G4" s="26">
         <v>43167</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H4" s="26">
         <v>43176</v>
       </c>
-      <c r="I4" s="29"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="27"/>
+      <c r="J4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="30"/>
+      <c r="K4" s="28"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="31" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="28">
+      <c r="F5" s="29"/>
+      <c r="G5" s="26">
         <v>43175</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="26">
         <v>43176</v>
       </c>
-      <c r="I5" s="29"/>
-      <c r="J5" s="11" t="s">
+      <c r="I5" s="27"/>
+      <c r="J5" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="K5" s="30"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="28">
+      <c r="F6" s="30"/>
+      <c r="G6" s="26">
         <v>43176</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="26">
         <v>43176</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="J6" s="11" t="s">
+      <c r="I6" s="27"/>
+      <c r="J6" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="30"/>
+      <c r="K6" s="28"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="28">
+      <c r="F7" s="28"/>
+      <c r="G7" s="26">
         <v>43176</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="26">
         <v>43176</v>
       </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="11" t="s">
+      <c r="I7" s="27"/>
+      <c r="J7" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="30"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11" t="s">
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="K8" s="30"/>
+      <c r="K8" s="28"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="1">
@@ -1241,8 +1301,8 @@
       <c r="H10" s="6">
         <v>43176</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="12" t="s">
+      <c r="I10" s="16"/>
+      <c r="J10" s="11" t="s">
         <v>79</v>
       </c>
       <c r="K10" s="1"/>
@@ -1268,8 +1328,8 @@
       <c r="H11" s="6">
         <v>43176</v>
       </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="16" t="s">
+      <c r="I11" s="16"/>
+      <c r="J11" s="15" t="s">
         <v>81</v>
       </c>
       <c r="K11" s="1"/>
@@ -1295,8 +1355,8 @@
       <c r="H12" s="6">
         <v>43176</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="16" t="s">
+      <c r="I12" s="16"/>
+      <c r="J12" s="15" t="s">
         <v>81</v>
       </c>
       <c r="K12" s="1"/>
@@ -1322,8 +1382,8 @@
       <c r="H13" s="6">
         <v>43176</v>
       </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="16" t="s">
+      <c r="I13" s="16"/>
+      <c r="J13" s="15" t="s">
         <v>81</v>
       </c>
       <c r="K13" s="1"/>
@@ -1349,8 +1409,8 @@
       <c r="H14" s="6">
         <v>43176</v>
       </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="16" t="s">
+      <c r="I14" s="16"/>
+      <c r="J14" s="15" t="s">
         <v>81</v>
       </c>
       <c r="K14" s="1"/>
@@ -1391,8 +1451,8 @@
       <c r="H16" s="6">
         <v>43177</v>
       </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="14" t="s">
+      <c r="I16" s="16"/>
+      <c r="J16" s="13" t="s">
         <v>92</v>
       </c>
       <c r="K16" s="1"/>
@@ -1418,8 +1478,8 @@
       <c r="H17" s="6">
         <v>43177</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="14" t="s">
+      <c r="I17" s="16"/>
+      <c r="J17" s="13" t="s">
         <v>92</v>
       </c>
       <c r="K17" s="1"/>
@@ -1445,8 +1505,8 @@
       <c r="H18" s="6">
         <v>43177</v>
       </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="14" t="s">
+      <c r="I18" s="16"/>
+      <c r="J18" s="13" t="s">
         <v>92</v>
       </c>
       <c r="K18" s="1"/>
@@ -1472,8 +1532,8 @@
       <c r="H19" s="6">
         <v>43177</v>
       </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="14" t="s">
+      <c r="I19" s="16"/>
+      <c r="J19" s="13" t="s">
         <v>92</v>
       </c>
       <c r="K19" s="1"/>
@@ -1499,8 +1559,8 @@
       <c r="H20" s="6">
         <v>43177</v>
       </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="14" t="s">
+      <c r="I20" s="16"/>
+      <c r="J20" s="13" t="s">
         <v>92</v>
       </c>
       <c r="K20" s="1"/>
@@ -1517,7 +1577,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="13" t="s">
         <v>92</v>
       </c>
       <c r="K21" s="1"/>
@@ -1526,463 +1586,463 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21">
+      <c r="F22" s="18"/>
+      <c r="G22" s="19">
         <v>43179</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="19">
         <v>43181</v>
       </c>
-      <c r="I22" s="22"/>
-      <c r="J22" s="13" t="s">
+      <c r="I22" s="20"/>
+      <c r="J22" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K22" s="23"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="21">
+      <c r="F23" s="21"/>
+      <c r="G23" s="19">
         <v>43179</v>
       </c>
-      <c r="H23" s="21">
+      <c r="H23" s="19">
         <v>43183</v>
       </c>
-      <c r="I23" s="22"/>
-      <c r="J23" s="13" t="s">
+      <c r="I23" s="20"/>
+      <c r="J23" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K23" s="23"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24" t="s">
+      <c r="B24" s="21"/>
+      <c r="C24" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="21">
+      <c r="F24" s="21"/>
+      <c r="G24" s="19">
         <v>43179</v>
       </c>
-      <c r="H24" s="21">
+      <c r="H24" s="19">
         <v>43183</v>
       </c>
-      <c r="I24" s="22"/>
-      <c r="J24" s="13" t="s">
+      <c r="I24" s="20"/>
+      <c r="J24" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="23"/>
+      <c r="K24" s="21"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="25" t="s">
+      <c r="B25" s="21"/>
+      <c r="C25" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="21">
+      <c r="F25" s="23"/>
+      <c r="G25" s="19">
         <v>43183</v>
       </c>
-      <c r="H25" s="21">
+      <c r="H25" s="19">
         <v>43183</v>
       </c>
-      <c r="I25" s="22"/>
-      <c r="J25" s="13" t="s">
+      <c r="I25" s="20"/>
+      <c r="J25" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K25" s="23"/>
+      <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23" t="s">
+      <c r="B26" s="21"/>
+      <c r="C26" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="21">
+      <c r="F26" s="21"/>
+      <c r="G26" s="19">
         <v>43183</v>
       </c>
-      <c r="H26" s="21">
+      <c r="H26" s="19">
         <v>43183</v>
       </c>
-      <c r="I26" s="22"/>
-      <c r="J26" s="13" t="s">
+      <c r="I26" s="20"/>
+      <c r="J26" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K26" s="23"/>
+      <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="22"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="23"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="20" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21">
+      <c r="F28" s="18"/>
+      <c r="G28" s="19">
         <v>43183</v>
       </c>
-      <c r="H28" s="21">
+      <c r="H28" s="19">
         <v>43183</v>
       </c>
-      <c r="I28" s="22"/>
-      <c r="J28" s="13" t="s">
+      <c r="I28" s="20"/>
+      <c r="J28" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K28" s="23"/>
+      <c r="K28" s="21"/>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="23"/>
-      <c r="G29" s="21">
+      <c r="F29" s="21"/>
+      <c r="G29" s="19">
         <v>43183</v>
       </c>
-      <c r="H29" s="21">
+      <c r="H29" s="19">
         <v>43183</v>
       </c>
-      <c r="I29" s="22"/>
-      <c r="J29" s="13" t="s">
+      <c r="I29" s="20"/>
+      <c r="J29" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K29" s="23"/>
+      <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="21">
+      <c r="F30" s="21"/>
+      <c r="G30" s="19">
         <v>43183</v>
       </c>
-      <c r="H30" s="21">
+      <c r="H30" s="19">
         <v>43183</v>
       </c>
-      <c r="I30" s="22"/>
-      <c r="J30" s="13" t="s">
+      <c r="I30" s="20"/>
+      <c r="J30" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K30" s="23"/>
+      <c r="K30" s="21"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="25" t="s">
+      <c r="B31" s="21"/>
+      <c r="C31" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="21">
+      <c r="F31" s="23"/>
+      <c r="G31" s="19">
         <v>43183</v>
       </c>
-      <c r="H31" s="21">
+      <c r="H31" s="19">
         <v>43183</v>
       </c>
-      <c r="I31" s="22"/>
-      <c r="J31" s="13" t="s">
+      <c r="I31" s="20"/>
+      <c r="J31" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K31" s="23"/>
+      <c r="K31" s="21"/>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23" t="s">
+      <c r="B32" s="21"/>
+      <c r="C32" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="23"/>
-      <c r="G32" s="21">
+      <c r="F32" s="21"/>
+      <c r="G32" s="19">
         <v>43183</v>
       </c>
-      <c r="H32" s="21">
+      <c r="H32" s="19">
         <v>43183</v>
       </c>
-      <c r="I32" s="22"/>
-      <c r="J32" s="13" t="s">
+      <c r="I32" s="20"/>
+      <c r="J32" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K32" s="23"/>
+      <c r="K32" s="21"/>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="23"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="21"/>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="20" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21">
+      <c r="F34" s="18"/>
+      <c r="G34" s="19">
         <v>43183</v>
       </c>
-      <c r="H34" s="21">
+      <c r="H34" s="19">
         <v>43184</v>
       </c>
-      <c r="I34" s="22"/>
-      <c r="J34" s="13" t="s">
+      <c r="I34" s="20"/>
+      <c r="J34" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K34" s="23"/>
+      <c r="K34" s="21"/>
     </row>
     <row r="35" spans="1:11">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24" t="s">
+      <c r="B35" s="21"/>
+      <c r="C35" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="21">
+      <c r="F35" s="21"/>
+      <c r="G35" s="19">
         <v>43183</v>
       </c>
-      <c r="H35" s="21">
+      <c r="H35" s="19">
         <v>43184</v>
       </c>
-      <c r="I35" s="22"/>
-      <c r="J35" s="13" t="s">
+      <c r="I35" s="20"/>
+      <c r="J35" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K35" s="23"/>
+      <c r="K35" s="21"/>
     </row>
     <row r="36" spans="1:11">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24" t="s">
+      <c r="B36" s="21"/>
+      <c r="C36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="23"/>
-      <c r="G36" s="21">
+      <c r="F36" s="21"/>
+      <c r="G36" s="19">
         <v>43184</v>
       </c>
-      <c r="H36" s="21">
+      <c r="H36" s="19">
         <v>43184</v>
       </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="13" t="s">
+      <c r="I36" s="20"/>
+      <c r="J36" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K36" s="23"/>
+      <c r="K36" s="21"/>
     </row>
     <row r="37" spans="1:11">
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="25" t="s">
+      <c r="B37" s="21"/>
+      <c r="C37" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="21">
+      <c r="F37" s="23"/>
+      <c r="G37" s="19">
         <v>43184</v>
       </c>
-      <c r="H37" s="21">
+      <c r="H37" s="19">
         <v>43184</v>
       </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="13" t="s">
+      <c r="I37" s="20"/>
+      <c r="J37" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K37" s="23"/>
+      <c r="K37" s="21"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="21">
+      <c r="F38" s="21"/>
+      <c r="G38" s="19">
         <v>43184</v>
       </c>
-      <c r="H38" s="21">
+      <c r="H38" s="19">
         <v>43184</v>
       </c>
-      <c r="I38" s="22"/>
-      <c r="J38" s="13" t="s">
+      <c r="I38" s="20"/>
+      <c r="J38" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K38" s="23"/>
+      <c r="K38" s="21"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23" t="s">
+      <c r="B39" s="21"/>
+      <c r="C39" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D39" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="23"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="21">
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="19">
         <v>43184</v>
       </c>
-      <c r="H39" s="21">
+      <c r="H39" s="19">
         <v>43184</v>
       </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="13" t="s">
+      <c r="I39" s="19"/>
+      <c r="J39" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="K39" s="23"/>
+      <c r="K39" s="21"/>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="1"/>
@@ -2022,7 +2082,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2035,14 +2095,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
@@ -2212,7 +2272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2227,22 +2287,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2253,16 +2313,16 @@
       <c r="B2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="36"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="1">
@@ -2271,16 +2331,16 @@
       <c r="B3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="36"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:7" ht="30">
       <c r="A4" s="1">
@@ -2289,16 +2349,16 @@
       <c r="B4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="36" t="s">
         <v>110</v>
       </c>
       <c r="G4" t="s">
@@ -2312,16 +2372,16 @@
       <c r="B5" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="37"/>
       <c r="G5" t="s">
         <v>116</v>
       </c>
@@ -2333,39 +2393,39 @@
       <c r="B6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="36" t="s">
         <v>110</v>
       </c>
       <c r="G6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
@@ -2374,14 +2434,14 @@
       <c r="B8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37" t="s">
+      <c r="D8" s="34"/>
+      <c r="E8" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="37"/>
       <c r="G8" t="s">
         <v>129</v>
       </c>
@@ -2390,9 +2450,9 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
@@ -2404,9 +2464,9 @@
       <c r="C10" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="39" t="s">
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="37" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2414,9 +2474,9 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
@@ -2428,29 +2488,29 @@
       <c r="C12" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="F12" s="36"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1"/>
@@ -2458,17 +2518,17 @@
       <c r="C15" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1"/>
@@ -2498,7 +2558,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="40"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
@@ -2713,4 +2773,317 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="34"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" ht="30">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="34"/>
+    </row>
+    <row r="12" spans="1:4" ht="23.25" customHeight="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30">
+      <c r="A1" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>